<commit_message>
Added a vanilla implementation of an object tracker using openCV's tracking API
</commit_message>
<xml_diff>
--- a/csvs/logs.09282017/brisk_flann_knn.xlsx
+++ b/csvs/logs.09282017/brisk_flann_knn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="-23220" windowWidth="18220" windowHeight="18280" tabRatio="500"/>
+    <workbookView xWindow="15080" yWindow="-22880" windowWidth="18180" windowHeight="17520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="brisk_flann_knn_with_match" sheetId="1" r:id="rId1"/>
@@ -1470,13 +1470,11 @@
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="00B050"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2122,7 +2120,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
+                  <a:schemeClr val="accent6">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -5357,6 +5355,7 @@
         <c:axId val="-264288176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5374,6 +5373,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times" charset="0"/>
+                    <a:ea typeface="Times" charset="0"/>
+                    <a:cs typeface="Times" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Ratio of Query/Train descriptors</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times" charset="0"/>
+                  <a:ea typeface="Times" charset="0"/>
+                  <a:cs typeface="Times" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5418,6 +5478,7 @@
         <c:axId val="-291803056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5435,6 +5496,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times" charset="0"/>
+                    <a:ea typeface="Times" charset="0"/>
+                    <a:cs typeface="Times" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times" charset="0"/>
+                  <a:ea typeface="Times" charset="0"/>
+                  <a:cs typeface="Times" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6116,16 +6238,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9829,7 +9951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="82" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B105"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Creating an object detector using contours.
</commit_message>
<xml_diff>
--- a/csvs/logs.09282017/brisk_flann_knn.xlsx
+++ b/csvs/logs.09282017/brisk_flann_knn.xlsx
@@ -9,16 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="-22880" windowWidth="18180" windowHeight="17520" tabRatio="500"/>
+    <workbookView xWindow="13200" yWindow="-22860" windowWidth="18180" windowHeight="17520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="brisk_flann_knn_with_match" sheetId="1" r:id="rId1"/>
     <sheet name="brisk_flann_knn_no_match" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -152,7 +149,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.138072398051411"/>
+          <c:y val="0.0255268676781256"/>
+          <c:w val="0.819612426851313"/>
+          <c:h val="0.77392679085846"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -5348,11 +5355,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-264288176"/>
-        <c:axId val="-291803056"/>
+        <c:axId val="1901486592"/>
+        <c:axId val="1859088560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-264288176"/>
+        <c:axId val="1901486592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -5470,12 +5477,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-291803056"/>
+        <c:crossAx val="1859088560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-291803056"/>
+        <c:axId val="1859088560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.45"/>
@@ -5593,7 +5600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-264288176"/>
+        <c:crossAx val="1901486592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5607,7 +5614,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.124616563007445"/>
+          <c:y val="0.902426118686384"/>
+          <c:w val="0.838315512117405"/>
+          <c:h val="0.0761104666794699"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5646,12 +5662,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -6239,15 +6250,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6267,3423 +6278,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="sift_flann_knn_with_match"/>
-      <sheetName val="sift_flann_knn_no_match"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="B6">
-            <v>0.12228</v>
-          </cell>
-          <cell r="C6">
-            <v>0.15908</v>
-          </cell>
-          <cell r="D6">
-            <v>7.6999999999999996E-4</v>
-          </cell>
-          <cell r="E6">
-            <v>3.0699999999999998E-3</v>
-          </cell>
-          <cell r="L6">
-            <v>0.27210031347962382</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.12393</v>
-          </cell>
-          <cell r="C7">
-            <v>0.16164999999999999</v>
-          </cell>
-          <cell r="D7">
-            <v>1E-3</v>
-          </cell>
-          <cell r="E7">
-            <v>4.5399999999999998E-3</v>
-          </cell>
-          <cell r="L7">
-            <v>0.26739811912225703</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.12103999999999999</v>
-          </cell>
-          <cell r="C8">
-            <v>0.18923000000000001</v>
-          </cell>
-          <cell r="D8">
-            <v>7.7999999999999999E-4</v>
-          </cell>
-          <cell r="E8">
-            <v>9.6299999999999997E-3</v>
-          </cell>
-          <cell r="L8">
-            <v>0.27272727272727271</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0.12121</v>
-          </cell>
-          <cell r="C9">
-            <v>0.16717000000000001</v>
-          </cell>
-          <cell r="D9">
-            <v>7.2999999999999996E-4</v>
-          </cell>
-          <cell r="E9">
-            <v>2.8999999999999998E-3</v>
-          </cell>
-          <cell r="L9">
-            <v>0.25956112852664576</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0.11891</v>
-          </cell>
-          <cell r="C10">
-            <v>0.16169</v>
-          </cell>
-          <cell r="D10">
-            <v>6.7000000000000002E-4</v>
-          </cell>
-          <cell r="E10">
-            <v>3.32E-3</v>
-          </cell>
-          <cell r="L10">
-            <v>0.27523510971786835</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0.12556999999999999</v>
-          </cell>
-          <cell r="C11">
-            <v>0.18064</v>
-          </cell>
-          <cell r="D11">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E11">
-            <v>2.7299999999999998E-3</v>
-          </cell>
-          <cell r="L11">
-            <v>0.30250783699059564</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>0.1241</v>
-          </cell>
-          <cell r="C12">
-            <v>0.15690999999999999</v>
-          </cell>
-          <cell r="D12">
-            <v>6.7000000000000002E-4</v>
-          </cell>
-          <cell r="E12">
-            <v>3.1099999999999999E-3</v>
-          </cell>
-          <cell r="L12">
-            <v>0.27899686520376177</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>0.12892999999999999</v>
-          </cell>
-          <cell r="C13">
-            <v>0.16933999999999999</v>
-          </cell>
-          <cell r="D13">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E13">
-            <v>2.7799999999999999E-3</v>
-          </cell>
-          <cell r="L13">
-            <v>0.30219435736677114</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>0.11726</v>
-          </cell>
-          <cell r="C14">
-            <v>0.16058</v>
-          </cell>
-          <cell r="D14">
-            <v>8.0999999999999996E-4</v>
-          </cell>
-          <cell r="E14">
-            <v>3.5100000000000001E-3</v>
-          </cell>
-          <cell r="L14">
-            <v>0.27962382445141065</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>0.10242999999999999</v>
-          </cell>
-          <cell r="C15">
-            <v>0.12152</v>
-          </cell>
-          <cell r="D15">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E15">
-            <v>3.62E-3</v>
-          </cell>
-          <cell r="L15">
-            <v>0.21410658307210031</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>0.10385</v>
-          </cell>
-          <cell r="C16">
-            <v>0.12881999999999999</v>
-          </cell>
-          <cell r="D16">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E16">
-            <v>3.2100000000000002E-3</v>
-          </cell>
-          <cell r="L16">
-            <v>0.22351097178683385</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>0.10706</v>
-          </cell>
-          <cell r="C17">
-            <v>0.13300000000000001</v>
-          </cell>
-          <cell r="D17">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E17">
-            <v>4.1200000000000004E-3</v>
-          </cell>
-          <cell r="L17">
-            <v>0.21630094043887146</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>0.125</v>
-          </cell>
-          <cell r="C18">
-            <v>0.18021999999999999</v>
-          </cell>
-          <cell r="D18">
-            <v>7.6000000000000004E-4</v>
-          </cell>
-          <cell r="E18">
-            <v>4.6100000000000004E-3</v>
-          </cell>
-          <cell r="L18">
-            <v>0.28401253918495301</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>0.11960999999999999</v>
-          </cell>
-          <cell r="C19">
-            <v>0.14373</v>
-          </cell>
-          <cell r="D19">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E19">
-            <v>6.0200000000000002E-3</v>
-          </cell>
-          <cell r="L19">
-            <v>0.23291536050156739</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>0.11608</v>
-          </cell>
-          <cell r="C20">
-            <v>0.14584</v>
-          </cell>
-          <cell r="D20">
-            <v>9.5E-4</v>
-          </cell>
-          <cell r="E20">
-            <v>3.0200000000000001E-3</v>
-          </cell>
-          <cell r="L20">
-            <v>0.23730407523510971</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>0.11859</v>
-          </cell>
-          <cell r="C21">
-            <v>0.14563000000000001</v>
-          </cell>
-          <cell r="D21">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E21">
-            <v>7.1700000000000002E-3</v>
-          </cell>
-          <cell r="L21">
-            <v>0.23479623824451409</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>0.13000999999999999</v>
-          </cell>
-          <cell r="C22">
-            <v>0.16786999999999999</v>
-          </cell>
-          <cell r="D22">
-            <v>7.1000000000000002E-4</v>
-          </cell>
-          <cell r="E22">
-            <v>3.13E-3</v>
-          </cell>
-          <cell r="L22">
-            <v>0.28934169278996863</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>0.12819</v>
-          </cell>
-          <cell r="C23">
-            <v>0.18013000000000001</v>
-          </cell>
-          <cell r="D23">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E23">
-            <v>2.5799999999999998E-3</v>
-          </cell>
-          <cell r="L23">
-            <v>0.30062695924764893</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>0.12786</v>
-          </cell>
-          <cell r="C24">
-            <v>0.19406000000000001</v>
-          </cell>
-          <cell r="D24">
-            <v>1.24E-3</v>
-          </cell>
-          <cell r="E24">
-            <v>7.8300000000000002E-3</v>
-          </cell>
-          <cell r="L24">
-            <v>0.30156739811912225</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>0.12454999999999999</v>
-          </cell>
-          <cell r="C25">
-            <v>0.16636000000000001</v>
-          </cell>
-          <cell r="D25">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E25">
-            <v>2.2699999999999999E-3</v>
-          </cell>
-          <cell r="L25">
-            <v>0.28056426332288403</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>0.11211</v>
-          </cell>
-          <cell r="C26">
-            <v>0.15831000000000001</v>
-          </cell>
-          <cell r="D26">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E26">
-            <v>2.49E-3</v>
-          </cell>
-          <cell r="L26">
-            <v>0.24733542319749216</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>0.11441</v>
-          </cell>
-          <cell r="C27">
-            <v>0.15185999999999999</v>
-          </cell>
-          <cell r="D27">
-            <v>9.3999999999999997E-4</v>
-          </cell>
-          <cell r="E27">
-            <v>6.3400000000000001E-3</v>
-          </cell>
-          <cell r="L27">
-            <v>0.24043887147335424</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>0.11074000000000001</v>
-          </cell>
-          <cell r="C28">
-            <v>0.14559</v>
-          </cell>
-          <cell r="D28">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E28">
-            <v>3.6099999999999999E-3</v>
-          </cell>
-          <cell r="L28">
-            <v>0.22852664576802509</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>0.11686000000000001</v>
-          </cell>
-          <cell r="C29">
-            <v>0.13639999999999999</v>
-          </cell>
-          <cell r="D29">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E29">
-            <v>5.0400000000000002E-3</v>
-          </cell>
-          <cell r="L29">
-            <v>0.23542319749216301</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>0.11823</v>
-          </cell>
-          <cell r="C30">
-            <v>0.15015000000000001</v>
-          </cell>
-          <cell r="D30">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E30">
-            <v>4.0899999999999999E-3</v>
-          </cell>
-          <cell r="L30">
-            <v>0.24827586206896551</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>0.12446</v>
-          </cell>
-          <cell r="C31">
-            <v>0.16224</v>
-          </cell>
-          <cell r="D31">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E31">
-            <v>3.0599999999999998E-3</v>
-          </cell>
-          <cell r="L31">
-            <v>0.26833855799373041</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>0.12329</v>
-          </cell>
-          <cell r="C32">
-            <v>0.16299</v>
-          </cell>
-          <cell r="D32">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E32">
-            <v>5.1700000000000001E-3</v>
-          </cell>
-          <cell r="L32">
-            <v>0.25203761755485893</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>0.12026000000000001</v>
-          </cell>
-          <cell r="C33">
-            <v>0.14671999999999999</v>
-          </cell>
-          <cell r="D33">
-            <v>7.2999999999999996E-4</v>
-          </cell>
-          <cell r="E33">
-            <v>3.1099999999999999E-3</v>
-          </cell>
-          <cell r="L33">
-            <v>0.24482758620689654</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>0.10864</v>
-          </cell>
-          <cell r="C34">
-            <v>0.15787000000000001</v>
-          </cell>
-          <cell r="D34">
-            <v>7.2000000000000005E-4</v>
-          </cell>
-          <cell r="E34">
-            <v>1.1390000000000001E-2</v>
-          </cell>
-          <cell r="L34">
-            <v>0.24827586206896551</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>0.113</v>
-          </cell>
-          <cell r="C35">
-            <v>0.14135</v>
-          </cell>
-          <cell r="D35">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E35">
-            <v>8.6199999999999992E-3</v>
-          </cell>
-          <cell r="L35">
-            <v>0.24576802507836989</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>0.12116</v>
-          </cell>
-          <cell r="C36">
-            <v>0.14792</v>
-          </cell>
-          <cell r="D36">
-            <v>7.2000000000000005E-4</v>
-          </cell>
-          <cell r="E36">
-            <v>6.3499999999999997E-3</v>
-          </cell>
-          <cell r="L36">
-            <v>0.24420062695924766</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>0.10854</v>
-          </cell>
-          <cell r="C37">
-            <v>0.13094</v>
-          </cell>
-          <cell r="D37">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E37">
-            <v>7.0699999999999999E-3</v>
-          </cell>
-          <cell r="L37">
-            <v>0.22570532915360503</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>0.12012</v>
-          </cell>
-          <cell r="C38">
-            <v>0.15254999999999999</v>
-          </cell>
-          <cell r="D38">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E38">
-            <v>3.0899999999999999E-3</v>
-          </cell>
-          <cell r="L38">
-            <v>0.25141065830721004</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>0.10680000000000001</v>
-          </cell>
-          <cell r="C39">
-            <v>0.13761999999999999</v>
-          </cell>
-          <cell r="D39">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E39">
-            <v>4.7400000000000003E-3</v>
-          </cell>
-          <cell r="L39">
-            <v>0.21065830721003134</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>0.10535</v>
-          </cell>
-          <cell r="C40">
-            <v>0.14474999999999999</v>
-          </cell>
-          <cell r="D40">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E40">
-            <v>7.0299999999999998E-3</v>
-          </cell>
-          <cell r="L40">
-            <v>0.20877742946708464</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>0.11845</v>
-          </cell>
-          <cell r="C41">
-            <v>0.13729</v>
-          </cell>
-          <cell r="D41">
-            <v>7.1000000000000002E-4</v>
-          </cell>
-          <cell r="E41">
-            <v>6.4200000000000004E-3</v>
-          </cell>
-          <cell r="L41">
-            <v>0.2225705329153605</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>0.11903</v>
-          </cell>
-          <cell r="C42">
-            <v>0.14896999999999999</v>
-          </cell>
-          <cell r="D42">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E42">
-            <v>2.32E-3</v>
-          </cell>
-          <cell r="L42">
-            <v>0.24075235109717869</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>0.11699</v>
-          </cell>
-          <cell r="C43">
-            <v>0.16475999999999999</v>
-          </cell>
-          <cell r="D43">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E43">
-            <v>3.62E-3</v>
-          </cell>
-          <cell r="L43">
-            <v>0.26081504702194358</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>0.12113</v>
-          </cell>
-          <cell r="C44">
-            <v>0.17452000000000001</v>
-          </cell>
-          <cell r="D44">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E44">
-            <v>1.094E-2</v>
-          </cell>
-          <cell r="L44">
-            <v>0.27836990595611283</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>0.11698</v>
-          </cell>
-          <cell r="C45">
-            <v>0.19463</v>
-          </cell>
-          <cell r="D45">
-            <v>9.8999999999999999E-4</v>
-          </cell>
-          <cell r="E45">
-            <v>3.46E-3</v>
-          </cell>
-          <cell r="L45">
-            <v>0.28902821316614419</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>0.12185</v>
-          </cell>
-          <cell r="C46">
-            <v>0.18572</v>
-          </cell>
-          <cell r="D46">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E46">
-            <v>2.5200000000000001E-3</v>
-          </cell>
-          <cell r="L46">
-            <v>0.30219435736677114</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>0.12697</v>
-          </cell>
-          <cell r="C47">
-            <v>0.20566999999999999</v>
-          </cell>
-          <cell r="D47">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E47">
-            <v>5.2900000000000004E-3</v>
-          </cell>
-          <cell r="L47">
-            <v>0.31786833855799373</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>0.12623999999999999</v>
-          </cell>
-          <cell r="C48">
-            <v>0.19938</v>
-          </cell>
-          <cell r="D48">
-            <v>1.9400000000000001E-3</v>
-          </cell>
-          <cell r="E48">
-            <v>7.6E-3</v>
-          </cell>
-          <cell r="L48">
-            <v>0.30470219435736678</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>0.11615</v>
-          </cell>
-          <cell r="C49">
-            <v>0.16292999999999999</v>
-          </cell>
-          <cell r="D49">
-            <v>3.49E-3</v>
-          </cell>
-          <cell r="E49">
-            <v>3.63E-3</v>
-          </cell>
-          <cell r="L49">
-            <v>0.27241379310344827</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>0.11745999999999999</v>
-          </cell>
-          <cell r="C50">
-            <v>0.16291</v>
-          </cell>
-          <cell r="D50">
-            <v>7.7999999999999999E-4</v>
-          </cell>
-          <cell r="E50">
-            <v>2.15E-3</v>
-          </cell>
-          <cell r="L50">
-            <v>0.24827586206896551</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>0.11903</v>
-          </cell>
-          <cell r="C51">
-            <v>0.18046000000000001</v>
-          </cell>
-          <cell r="D51">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E51">
-            <v>2.6900000000000001E-3</v>
-          </cell>
-          <cell r="L51">
-            <v>0.28996865203761757</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>0.13125999999999999</v>
-          </cell>
-          <cell r="C52">
-            <v>0.22500000000000001</v>
-          </cell>
-          <cell r="D52">
-            <v>7.3999999999999999E-4</v>
-          </cell>
-          <cell r="E52">
-            <v>2.8600000000000001E-3</v>
-          </cell>
-          <cell r="L52">
-            <v>0.33636363636363636</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>0.13905999999999999</v>
-          </cell>
-          <cell r="C53">
-            <v>0.19839999999999999</v>
-          </cell>
-          <cell r="D53">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E53">
-            <v>2.5200000000000001E-3</v>
-          </cell>
-          <cell r="L53">
-            <v>0.32946708463949842</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>0.13428999999999999</v>
-          </cell>
-          <cell r="C54">
-            <v>0.22081999999999999</v>
-          </cell>
-          <cell r="D54">
-            <v>6.9999999999999999E-4</v>
-          </cell>
-          <cell r="E54">
-            <v>2.5699999999999998E-3</v>
-          </cell>
-          <cell r="L54">
-            <v>0.35297805642633229</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>0.14796999999999999</v>
-          </cell>
-          <cell r="C55">
-            <v>0.20824000000000001</v>
-          </cell>
-          <cell r="D55">
-            <v>1.73E-3</v>
-          </cell>
-          <cell r="E55">
-            <v>5.45E-3</v>
-          </cell>
-          <cell r="L55">
-            <v>0.34420062695924764</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>0.13028999999999999</v>
-          </cell>
-          <cell r="C56">
-            <v>0.23777999999999999</v>
-          </cell>
-          <cell r="D56">
-            <v>1.1199999999999999E-3</v>
-          </cell>
-          <cell r="E56">
-            <v>3.16E-3</v>
-          </cell>
-          <cell r="L56">
-            <v>0.3347962382445141</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>0.12734999999999999</v>
-          </cell>
-          <cell r="C57">
-            <v>0.21121000000000001</v>
-          </cell>
-          <cell r="D57">
-            <v>1.1299999999999999E-3</v>
-          </cell>
-          <cell r="E57">
-            <v>4.47E-3</v>
-          </cell>
-          <cell r="L57">
-            <v>0.31786833855799373</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58">
-            <v>0.12053999999999999</v>
-          </cell>
-          <cell r="C58">
-            <v>0.17498</v>
-          </cell>
-          <cell r="D58">
-            <v>6.7000000000000002E-4</v>
-          </cell>
-          <cell r="E58">
-            <v>2.9299999999999999E-3</v>
-          </cell>
-          <cell r="L58">
-            <v>0.27868338557993733</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59">
-            <v>0.12659000000000001</v>
-          </cell>
-          <cell r="C59">
-            <v>0.19725000000000001</v>
-          </cell>
-          <cell r="D59">
-            <v>9.3999999999999997E-4</v>
-          </cell>
-          <cell r="E59">
-            <v>2.98E-3</v>
-          </cell>
-          <cell r="L59">
-            <v>0.32319749216300941</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>0.12192</v>
-          </cell>
-          <cell r="C60">
-            <v>0.17043</v>
-          </cell>
-          <cell r="D60">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E60">
-            <v>4.9800000000000001E-3</v>
-          </cell>
-          <cell r="L60">
-            <v>0.29968652037617555</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61">
-            <v>0.11451</v>
-          </cell>
-          <cell r="C61">
-            <v>0.19081999999999999</v>
-          </cell>
-          <cell r="D61">
-            <v>8.1999999999999998E-4</v>
-          </cell>
-          <cell r="E61">
-            <v>5.3200000000000001E-3</v>
-          </cell>
-          <cell r="L61">
-            <v>0.28683385579937304</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62">
-            <v>0.12157999999999999</v>
-          </cell>
-          <cell r="C62">
-            <v>0.15801999999999999</v>
-          </cell>
-          <cell r="D62">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E62">
-            <v>2.5999999999999999E-3</v>
-          </cell>
-          <cell r="L62">
-            <v>0.26802507836990597</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="B63">
-            <v>0.12709999999999999</v>
-          </cell>
-          <cell r="C63">
-            <v>0.18124999999999999</v>
-          </cell>
-          <cell r="D63">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E63">
-            <v>6.6100000000000004E-3</v>
-          </cell>
-          <cell r="L63">
-            <v>0.3018808777429467</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64">
-            <v>0.13127</v>
-          </cell>
-          <cell r="C64">
-            <v>0.17416999999999999</v>
-          </cell>
-          <cell r="D64">
-            <v>1E-3</v>
-          </cell>
-          <cell r="E64">
-            <v>5.1799999999999997E-3</v>
-          </cell>
-          <cell r="L64">
-            <v>0.29498432601880875</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="B65">
-            <v>0.13031000000000001</v>
-          </cell>
-          <cell r="C65">
-            <v>0.19875999999999999</v>
-          </cell>
-          <cell r="D65">
-            <v>6.9999999999999999E-4</v>
-          </cell>
-          <cell r="E65">
-            <v>6.4200000000000004E-3</v>
-          </cell>
-          <cell r="L65">
-            <v>0.32601880877742945</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="B66">
-            <v>0.13199</v>
-          </cell>
-          <cell r="C66">
-            <v>0.17734</v>
-          </cell>
-          <cell r="D66">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E66">
-            <v>2.3400000000000001E-3</v>
-          </cell>
-          <cell r="L66">
-            <v>0.28526645768025077</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="B67">
-            <v>0.10228</v>
-          </cell>
-          <cell r="C67">
-            <v>0.11387</v>
-          </cell>
-          <cell r="D67">
-            <v>6.9999999999999999E-4</v>
-          </cell>
-          <cell r="E67">
-            <v>1.119E-2</v>
-          </cell>
-          <cell r="L67">
-            <v>0.1793103448275862</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="B68">
-            <v>0.11323</v>
-          </cell>
-          <cell r="C68">
-            <v>0.15090999999999999</v>
-          </cell>
-          <cell r="D68">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E68">
-            <v>5.5399999999999998E-3</v>
-          </cell>
-          <cell r="L68">
-            <v>0.23699059561128527</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69">
-            <v>0.11430999999999999</v>
-          </cell>
-          <cell r="C69">
-            <v>0.15898999999999999</v>
-          </cell>
-          <cell r="D69">
-            <v>7.9000000000000001E-4</v>
-          </cell>
-          <cell r="E69">
-            <v>3.64E-3</v>
-          </cell>
-          <cell r="L69">
-            <v>0.2413793103448276</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="B70">
-            <v>0.11394</v>
-          </cell>
-          <cell r="C70">
-            <v>0.15681</v>
-          </cell>
-          <cell r="D70">
-            <v>7.9000000000000001E-4</v>
-          </cell>
-          <cell r="E70">
-            <v>6.8900000000000003E-3</v>
-          </cell>
-          <cell r="L70">
-            <v>0.24576802507836989</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="B71">
-            <v>0.11987</v>
-          </cell>
-          <cell r="C71">
-            <v>0.1414</v>
-          </cell>
-          <cell r="D71">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E71">
-            <v>3.1700000000000001E-3</v>
-          </cell>
-          <cell r="L71">
-            <v>0.23322884012539186</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="B72">
-            <v>0.12595999999999999</v>
-          </cell>
-          <cell r="C72">
-            <v>0.15891</v>
-          </cell>
-          <cell r="D72">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E72">
-            <v>4.8599999999999997E-3</v>
-          </cell>
-          <cell r="L72">
-            <v>0.26708463949843259</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73">
-            <v>0.11624</v>
-          </cell>
-          <cell r="C73">
-            <v>0.17466000000000001</v>
-          </cell>
-          <cell r="D73">
-            <v>1.01E-3</v>
-          </cell>
-          <cell r="E73">
-            <v>8.8199999999999997E-3</v>
-          </cell>
-          <cell r="L73">
-            <v>0.26739811912225703</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="B74">
-            <v>0.11805</v>
-          </cell>
-          <cell r="C74">
-            <v>0.1754</v>
-          </cell>
-          <cell r="D74">
-            <v>7.1000000000000002E-4</v>
-          </cell>
-          <cell r="E74">
-            <v>2.7200000000000002E-3</v>
-          </cell>
-          <cell r="L74">
-            <v>0.26112852664576802</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="B75">
-            <v>0.11615</v>
-          </cell>
-          <cell r="C75">
-            <v>0.14668999999999999</v>
-          </cell>
-          <cell r="D75">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E75">
-            <v>3.31E-3</v>
-          </cell>
-          <cell r="L75">
-            <v>0.25423197492163008</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="B76">
-            <v>0.10886</v>
-          </cell>
-          <cell r="C76">
-            <v>0.15614</v>
-          </cell>
-          <cell r="D76">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E76">
-            <v>3.9500000000000004E-3</v>
-          </cell>
-          <cell r="L76">
-            <v>0.2476489028213166</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77">
-            <v>0.12092</v>
-          </cell>
-          <cell r="C77">
-            <v>0.15054999999999999</v>
-          </cell>
-          <cell r="D77">
-            <v>7.1000000000000002E-4</v>
-          </cell>
-          <cell r="E77">
-            <v>8.5000000000000006E-3</v>
-          </cell>
-          <cell r="L77">
-            <v>0.24388714733542319</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78">
-            <v>0.13167999999999999</v>
-          </cell>
-          <cell r="C78">
-            <v>0.16422</v>
-          </cell>
-          <cell r="D78">
-            <v>3.0200000000000001E-3</v>
-          </cell>
-          <cell r="E78">
-            <v>3.8899999999999998E-3</v>
-          </cell>
-          <cell r="L78">
-            <v>0.25924764890282131</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79">
-            <v>0.12664</v>
-          </cell>
-          <cell r="C79">
-            <v>0.16305</v>
-          </cell>
-          <cell r="D79">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E79">
-            <v>4.5700000000000003E-3</v>
-          </cell>
-          <cell r="L79">
-            <v>0.28244514106583074</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="B80">
-            <v>0.12597</v>
-          </cell>
-          <cell r="C80">
-            <v>0.18425</v>
-          </cell>
-          <cell r="D80">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E80">
-            <v>3.7100000000000002E-3</v>
-          </cell>
-          <cell r="L80">
-            <v>0.29090909090909089</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="B81">
-            <v>0.12444</v>
-          </cell>
-          <cell r="C81">
-            <v>0.18698000000000001</v>
-          </cell>
-          <cell r="D81">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E81">
-            <v>3.9300000000000003E-3</v>
-          </cell>
-          <cell r="L81">
-            <v>0.29122257053291534</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="B82">
-            <v>0.11183</v>
-          </cell>
-          <cell r="C82">
-            <v>0.13880999999999999</v>
-          </cell>
-          <cell r="D82">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E82">
-            <v>1.3299999999999999E-2</v>
-          </cell>
-          <cell r="L82">
-            <v>0.22884012539184953</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83">
-            <v>0.11024</v>
-          </cell>
-          <cell r="C83">
-            <v>0.11337</v>
-          </cell>
-          <cell r="D83">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E83">
-            <v>9.5999999999999992E-3</v>
-          </cell>
-          <cell r="L83">
-            <v>0.1915360501567398</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84">
-            <v>9.8379999999999995E-2</v>
-          </cell>
-          <cell r="C84">
-            <v>0.10857</v>
-          </cell>
-          <cell r="D84">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E84">
-            <v>1.1849999999999999E-2</v>
-          </cell>
-          <cell r="L84">
-            <v>0.17210031347962382</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85">
-            <v>0.11756999999999999</v>
-          </cell>
-          <cell r="C85">
-            <v>0.16205</v>
-          </cell>
-          <cell r="D85">
-            <v>8.8999999999999995E-4</v>
-          </cell>
-          <cell r="E85">
-            <v>5.4000000000000003E-3</v>
-          </cell>
-          <cell r="L85">
-            <v>0.26238244514106585</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="B86">
-            <v>0.10604</v>
-          </cell>
-          <cell r="C86">
-            <v>0.12639</v>
-          </cell>
-          <cell r="D86">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E86">
-            <v>2.5000000000000001E-3</v>
-          </cell>
-          <cell r="L86">
-            <v>0.21191222570532917</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87">
-            <v>0.10826</v>
-          </cell>
-          <cell r="C87">
-            <v>0.15290999999999999</v>
-          </cell>
-          <cell r="D87">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E87">
-            <v>1.9499999999999999E-3</v>
-          </cell>
-          <cell r="L87">
-            <v>0.24827586206896551</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88">
-            <v>0.12386999999999999</v>
-          </cell>
-          <cell r="C88">
-            <v>0.16444</v>
-          </cell>
-          <cell r="D88">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E88">
-            <v>4.4000000000000003E-3</v>
-          </cell>
-          <cell r="L88">
-            <v>0.27868338557993733</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="B89">
-            <v>0.12631000000000001</v>
-          </cell>
-          <cell r="C89">
-            <v>0.19086</v>
-          </cell>
-          <cell r="D89">
-            <v>7.3999999999999999E-4</v>
-          </cell>
-          <cell r="E89">
-            <v>2.5400000000000002E-3</v>
-          </cell>
-          <cell r="L89">
-            <v>0.32006269592476488</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="B90">
-            <v>0.12250999999999999</v>
-          </cell>
-          <cell r="C90">
-            <v>0.17768</v>
-          </cell>
-          <cell r="D90">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E90">
-            <v>6.9300000000000004E-3</v>
-          </cell>
-          <cell r="L90">
-            <v>0.30094043887147337</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="B91">
-            <v>0.12397</v>
-          </cell>
-          <cell r="C91">
-            <v>0.18429000000000001</v>
-          </cell>
-          <cell r="D91">
-            <v>6.7000000000000002E-4</v>
-          </cell>
-          <cell r="E91">
-            <v>3.64E-3</v>
-          </cell>
-          <cell r="L91">
-            <v>0.30940438871473352</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="B92">
-            <v>0.11914</v>
-          </cell>
-          <cell r="C92">
-            <v>0.16933999999999999</v>
-          </cell>
-          <cell r="D92">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E92">
-            <v>3.6600000000000001E-3</v>
-          </cell>
-          <cell r="L92">
-            <v>0.2884012539184953</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="B93">
-            <v>0.1111</v>
-          </cell>
-          <cell r="C93">
-            <v>0.15214</v>
-          </cell>
-          <cell r="D93">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E93">
-            <v>4.6499999999999996E-3</v>
-          </cell>
-          <cell r="L93">
-            <v>0.26175548589341691</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="B94">
-            <v>0.10528999999999999</v>
-          </cell>
-          <cell r="C94">
-            <v>0.13663</v>
-          </cell>
-          <cell r="D94">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E94">
-            <v>3.0699999999999998E-3</v>
-          </cell>
-          <cell r="L94">
-            <v>0.2413793103448276</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="B95">
-            <v>0.11266</v>
-          </cell>
-          <cell r="C95">
-            <v>0.14324999999999999</v>
-          </cell>
-          <cell r="D95">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E95">
-            <v>5.6499999999999996E-3</v>
-          </cell>
-          <cell r="L95">
-            <v>0.22413793103448276</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="B96">
-            <v>0.1087</v>
-          </cell>
-          <cell r="C96">
-            <v>0.11570999999999999</v>
-          </cell>
-          <cell r="D96">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E96">
-            <v>1.8870000000000001E-2</v>
-          </cell>
-          <cell r="L96">
-            <v>0.20721003134796237</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="B97">
-            <v>0.10378</v>
-          </cell>
-          <cell r="C97">
-            <v>0.13622999999999999</v>
-          </cell>
-          <cell r="D97">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E97">
-            <v>1.1220000000000001E-2</v>
-          </cell>
-          <cell r="L97">
-            <v>0.21786833855799373</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="B98">
-            <v>0.10818999999999999</v>
-          </cell>
-          <cell r="C98">
-            <v>0.12584000000000001</v>
-          </cell>
-          <cell r="D98">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E98">
-            <v>6.8900000000000003E-3</v>
-          </cell>
-          <cell r="L98">
-            <v>0.21410658307210031</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="B99">
-            <v>9.9040000000000003E-2</v>
-          </cell>
-          <cell r="C99">
-            <v>0.12199</v>
-          </cell>
-          <cell r="D99">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E99">
-            <v>5.13E-3</v>
-          </cell>
-          <cell r="L99">
-            <v>0.20470219435736678</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="B100">
-            <v>0.10178</v>
-          </cell>
-          <cell r="C100">
-            <v>0.13292999999999999</v>
-          </cell>
-          <cell r="D100">
-            <v>7.2999999999999996E-4</v>
-          </cell>
-          <cell r="E100">
-            <v>5.9500000000000004E-3</v>
-          </cell>
-          <cell r="L100">
-            <v>0.21003134796238246</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="B101">
-            <v>0.10415000000000001</v>
-          </cell>
-          <cell r="C101">
-            <v>0.11724999999999999</v>
-          </cell>
-          <cell r="D101">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E101">
-            <v>3.7100000000000002E-3</v>
-          </cell>
-          <cell r="L101">
-            <v>0.19059561128526645</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="B102">
-            <v>0.10009999999999999</v>
-          </cell>
-          <cell r="C102">
-            <v>0.11874999999999999</v>
-          </cell>
-          <cell r="D102">
-            <v>9.3000000000000005E-4</v>
-          </cell>
-          <cell r="E102">
-            <v>4.9300000000000004E-3</v>
-          </cell>
-          <cell r="L102">
-            <v>0.19184952978056427</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="B103">
-            <v>9.8229999999999998E-2</v>
-          </cell>
-          <cell r="C103">
-            <v>0.11896</v>
-          </cell>
-          <cell r="D103">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E103">
-            <v>6.8700000000000002E-3</v>
-          </cell>
-          <cell r="L103">
-            <v>0.20626959247648902</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="B104">
-            <v>0.10607</v>
-          </cell>
-          <cell r="C104">
-            <v>0.13083</v>
-          </cell>
-          <cell r="D104">
-            <v>9.3000000000000005E-4</v>
-          </cell>
-          <cell r="E104">
-            <v>1.023E-2</v>
-          </cell>
-          <cell r="L104">
-            <v>0.21253918495297805</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="B105">
-            <v>0.10753</v>
-          </cell>
-          <cell r="C105">
-            <v>0.13533000000000001</v>
-          </cell>
-          <cell r="D105">
-            <v>3.1800000000000001E-3</v>
-          </cell>
-          <cell r="E105">
-            <v>5.5100000000000001E-3</v>
-          </cell>
-          <cell r="L105">
-            <v>0.21222570532915361</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="6">
-          <cell r="B6">
-            <v>8.7290000000000006E-2</v>
-          </cell>
-          <cell r="C6">
-            <v>6.0519999999999997E-2</v>
-          </cell>
-          <cell r="D6">
-            <v>7.6000000000000004E-4</v>
-          </cell>
-          <cell r="E6">
-            <v>1.35E-2</v>
-          </cell>
-          <cell r="L6">
-            <v>9.1849529780564265E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>8.3290000000000003E-2</v>
-          </cell>
-          <cell r="C7">
-            <v>7.46E-2</v>
-          </cell>
-          <cell r="D7">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E7">
-            <v>3.5720000000000002E-2</v>
-          </cell>
-          <cell r="L7">
-            <v>0.10626959247648902</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>8.0310000000000006E-2</v>
-          </cell>
-          <cell r="C8">
-            <v>6.4640000000000003E-2</v>
-          </cell>
-          <cell r="D8">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E8">
-            <v>6.8700000000000002E-3</v>
-          </cell>
-          <cell r="L8">
-            <v>0.1115987460815047</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>8.3659999999999998E-2</v>
-          </cell>
-          <cell r="C9">
-            <v>7.0809999999999998E-2</v>
-          </cell>
-          <cell r="D9">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E9">
-            <v>1.9699999999999999E-2</v>
-          </cell>
-          <cell r="L9">
-            <v>0.10532915360501567</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>8.2669999999999993E-2</v>
-          </cell>
-          <cell r="C10">
-            <v>6.7360000000000003E-2</v>
-          </cell>
-          <cell r="D10">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E10">
-            <v>6.4599999999999996E-3</v>
-          </cell>
-          <cell r="L10">
-            <v>0.10689655172413794</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>8.0850000000000005E-2</v>
-          </cell>
-          <cell r="C11">
-            <v>6.6460000000000005E-2</v>
-          </cell>
-          <cell r="D11">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E11">
-            <v>4.62E-3</v>
-          </cell>
-          <cell r="L11">
-            <v>9.968652037617555E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>8.6290000000000006E-2</v>
-          </cell>
-          <cell r="C12">
-            <v>7.9039999999999999E-2</v>
-          </cell>
-          <cell r="D12">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E12">
-            <v>3.2829999999999998E-2</v>
-          </cell>
-          <cell r="L12">
-            <v>0.11504702194357366</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>8.3460000000000006E-2</v>
-          </cell>
-          <cell r="C13">
-            <v>6.9870000000000002E-2</v>
-          </cell>
-          <cell r="D13">
-            <v>7.2999999999999996E-4</v>
-          </cell>
-          <cell r="E13">
-            <v>1.338E-2</v>
-          </cell>
-          <cell r="L13">
-            <v>0.10689655172413794</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>9.1480000000000006E-2</v>
-          </cell>
-          <cell r="C14">
-            <v>6.9769999999999999E-2</v>
-          </cell>
-          <cell r="D14">
-            <v>5.5999999999999995E-4</v>
-          </cell>
-          <cell r="E14">
-            <v>3.1699999999999999E-2</v>
-          </cell>
-          <cell r="L14">
-            <v>0.11347962382445141</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>8.6379999999999998E-2</v>
-          </cell>
-          <cell r="C15">
-            <v>7.5310000000000002E-2</v>
-          </cell>
-          <cell r="D15">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E15">
-            <v>3.2199999999999999E-2</v>
-          </cell>
-          <cell r="L15">
-            <v>0.11347962382445141</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>8.3699999999999997E-2</v>
-          </cell>
-          <cell r="C16">
-            <v>6.4339999999999994E-2</v>
-          </cell>
-          <cell r="D16">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E16">
-            <v>4.5900000000000003E-3</v>
-          </cell>
-          <cell r="L16">
-            <v>0.10846394984326019</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>8.4769999999999998E-2</v>
-          </cell>
-          <cell r="C17">
-            <v>6.6790000000000002E-2</v>
-          </cell>
-          <cell r="D17">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E17">
-            <v>7.79E-3</v>
-          </cell>
-          <cell r="L17">
-            <v>0.11097178683385579</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>8.2030000000000006E-2</v>
-          </cell>
-          <cell r="C18">
-            <v>6.361E-2</v>
-          </cell>
-          <cell r="D18">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E18">
-            <v>1.9E-3</v>
-          </cell>
-          <cell r="L18">
-            <v>0.10470219435736677</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>8.5150000000000003E-2</v>
-          </cell>
-          <cell r="C19">
-            <v>6.4640000000000003E-2</v>
-          </cell>
-          <cell r="D19">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E19">
-            <v>8.4399999999999996E-3</v>
-          </cell>
-          <cell r="L19">
-            <v>0.10313479623824451</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>8.6739999999999998E-2</v>
-          </cell>
-          <cell r="C20">
-            <v>7.3880000000000001E-2</v>
-          </cell>
-          <cell r="D20">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E20">
-            <v>1.0120000000000001E-2</v>
-          </cell>
-          <cell r="L20">
-            <v>0.11253918495297806</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>8.8469999999999993E-2</v>
-          </cell>
-          <cell r="C21">
-            <v>6.9199999999999998E-2</v>
-          </cell>
-          <cell r="D21">
-            <v>8.4999999999999995E-4</v>
-          </cell>
-          <cell r="E21">
-            <v>1.8489999999999999E-2</v>
-          </cell>
-          <cell r="L21">
-            <v>0.109717868338558</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>8.2600000000000007E-2</v>
-          </cell>
-          <cell r="C22">
-            <v>6.5820000000000004E-2</v>
-          </cell>
-          <cell r="D22">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E22">
-            <v>1.486E-2</v>
-          </cell>
-          <cell r="L22">
-            <v>0.109717868338558</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>8.2049999999999998E-2</v>
-          </cell>
-          <cell r="C23">
-            <v>6.6350000000000006E-2</v>
-          </cell>
-          <cell r="D23">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E23">
-            <v>3.82E-3</v>
-          </cell>
-          <cell r="L23">
-            <v>0.10689655172413794</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>8.7110000000000007E-2</v>
-          </cell>
-          <cell r="C24">
-            <v>7.3130000000000001E-2</v>
-          </cell>
-          <cell r="D24">
-            <v>1.0499999999999999E-3</v>
-          </cell>
-          <cell r="E24">
-            <v>3.4610000000000002E-2</v>
-          </cell>
-          <cell r="L24">
-            <v>0.10909090909090909</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>8.7359999999999993E-2</v>
-          </cell>
-          <cell r="C25">
-            <v>7.0069999999999993E-2</v>
-          </cell>
-          <cell r="D25">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E25">
-            <v>3.4020000000000002E-2</v>
-          </cell>
-          <cell r="L25">
-            <v>0.1122257053291536</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>8.3430000000000004E-2</v>
-          </cell>
-          <cell r="C26">
-            <v>6.3460000000000003E-2</v>
-          </cell>
-          <cell r="D26">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E26">
-            <v>1.5779999999999999E-2</v>
-          </cell>
-          <cell r="L26">
-            <v>0.10156739811912226</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>8.5360000000000005E-2</v>
-          </cell>
-          <cell r="C27">
-            <v>7.0599999999999996E-2</v>
-          </cell>
-          <cell r="D27">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E27">
-            <v>3.7920000000000002E-2</v>
-          </cell>
-          <cell r="L27">
-            <v>0.1103448275862069</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>8.1759999999999999E-2</v>
-          </cell>
-          <cell r="C28">
-            <v>6.6460000000000005E-2</v>
-          </cell>
-          <cell r="D28">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E28">
-            <v>3.2840000000000001E-2</v>
-          </cell>
-          <cell r="L28">
-            <v>0.11003134796238244</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>8.6900000000000005E-2</v>
-          </cell>
-          <cell r="C29">
-            <v>6.4769999999999994E-2</v>
-          </cell>
-          <cell r="D29">
-            <v>9.3000000000000005E-4</v>
-          </cell>
-          <cell r="E29">
-            <v>3.7249999999999998E-2</v>
-          </cell>
-          <cell r="L29">
-            <v>0.10344827586206896</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>8.1860000000000002E-2</v>
-          </cell>
-          <cell r="C30">
-            <v>6.0130000000000003E-2</v>
-          </cell>
-          <cell r="D30">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E30">
-            <v>4.7200000000000002E-3</v>
-          </cell>
-          <cell r="L30">
-            <v>9.7492163009404387E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>7.8109999999999999E-2</v>
-          </cell>
-          <cell r="C31">
-            <v>6.0850000000000001E-2</v>
-          </cell>
-          <cell r="D31">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E31">
-            <v>3.2390000000000002E-2</v>
-          </cell>
-          <cell r="L31">
-            <v>9.843260188087774E-2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>0.08</v>
-          </cell>
-          <cell r="C32">
-            <v>6.4180000000000001E-2</v>
-          </cell>
-          <cell r="D32">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E32">
-            <v>1.206E-2</v>
-          </cell>
-          <cell r="L32">
-            <v>9.968652037617555E-2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>9.962E-2</v>
-          </cell>
-          <cell r="C33">
-            <v>6.8309999999999996E-2</v>
-          </cell>
-          <cell r="D33">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E33">
-            <v>3.5200000000000001E-3</v>
-          </cell>
-          <cell r="L33">
-            <v>0.10783699059561129</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>8.3030000000000007E-2</v>
-          </cell>
-          <cell r="C34">
-            <v>6.1780000000000002E-2</v>
-          </cell>
-          <cell r="D34">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E34">
-            <v>9.5200000000000007E-3</v>
-          </cell>
-          <cell r="L34">
-            <v>0.10282131661442007</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>7.7679999999999999E-2</v>
-          </cell>
-          <cell r="C35">
-            <v>6.0060000000000002E-2</v>
-          </cell>
-          <cell r="D35">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E35">
-            <v>1.286E-2</v>
-          </cell>
-          <cell r="L35">
-            <v>0.10219435736677115</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>8.2580000000000001E-2</v>
-          </cell>
-          <cell r="C36">
-            <v>6.608E-2</v>
-          </cell>
-          <cell r="D36">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E36">
-            <v>3.9570000000000001E-2</v>
-          </cell>
-          <cell r="L36">
-            <v>0.10094043887147336</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>0.10359</v>
-          </cell>
-          <cell r="C37">
-            <v>6.862E-2</v>
-          </cell>
-          <cell r="D37">
-            <v>5.6999999999999998E-4</v>
-          </cell>
-          <cell r="E37">
-            <v>1.554E-2</v>
-          </cell>
-          <cell r="L37">
-            <v>0.1006269592476489</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>6.8529999999999994E-2</v>
-          </cell>
-          <cell r="C38">
-            <v>4.0779999999999997E-2</v>
-          </cell>
-          <cell r="D38">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E38">
-            <v>2.366E-2</v>
-          </cell>
-          <cell r="L38">
-            <v>6.2068965517241378E-2</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>7.1429999999999993E-2</v>
-          </cell>
-          <cell r="C39">
-            <v>5.0200000000000002E-2</v>
-          </cell>
-          <cell r="D39">
-            <v>1.97E-3</v>
-          </cell>
-          <cell r="E39">
-            <v>3.542E-2</v>
-          </cell>
-          <cell r="L39">
-            <v>7.6802507836990594E-2</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>6.8779999999999994E-2</v>
-          </cell>
-          <cell r="C40">
-            <v>4.2639999999999997E-2</v>
-          </cell>
-          <cell r="D40">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E40">
-            <v>1.4019999999999999E-2</v>
-          </cell>
-          <cell r="L40">
-            <v>6.9905956112852663E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>7.0879999999999999E-2</v>
-          </cell>
-          <cell r="C41">
-            <v>4.4540000000000003E-2</v>
-          </cell>
-          <cell r="D41">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E41">
-            <v>1.644E-2</v>
-          </cell>
-          <cell r="L41">
-            <v>6.8652037617554854E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>7.7649999999999997E-2</v>
-          </cell>
-          <cell r="C42">
-            <v>6.5879999999999994E-2</v>
-          </cell>
-          <cell r="D42">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E42">
-            <v>3.2960000000000003E-2</v>
-          </cell>
-          <cell r="L42">
-            <v>0.10595611285266458</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>8.4739999999999996E-2</v>
-          </cell>
-          <cell r="C43">
-            <v>6.1920000000000003E-2</v>
-          </cell>
-          <cell r="D43">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E43">
-            <v>9.5099999999999994E-3</v>
-          </cell>
-          <cell r="L43">
-            <v>0.10282131661442007</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>8.3769999999999997E-2</v>
-          </cell>
-          <cell r="C44">
-            <v>6.0810000000000003E-2</v>
-          </cell>
-          <cell r="D44">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E44">
-            <v>2.7210000000000002E-2</v>
-          </cell>
-          <cell r="L44">
-            <v>0.1006269592476489</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>7.7259999999999995E-2</v>
-          </cell>
-          <cell r="C45">
-            <v>5.4149999999999997E-2</v>
-          </cell>
-          <cell r="D45">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E45">
-            <v>2.5940000000000001E-2</v>
-          </cell>
-          <cell r="L45">
-            <v>8.526645768025079E-2</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>7.8299999999999995E-2</v>
-          </cell>
-          <cell r="C46">
-            <v>4.2000000000000003E-2</v>
-          </cell>
-          <cell r="D46">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E46">
-            <v>8.6300000000000005E-3</v>
-          </cell>
-          <cell r="L46">
-            <v>6.6771159874608146E-2</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>7.2480000000000003E-2</v>
-          </cell>
-          <cell r="C47">
-            <v>4.879E-2</v>
-          </cell>
-          <cell r="D47">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E47">
-            <v>2.0699999999999998E-3</v>
-          </cell>
-          <cell r="L47">
-            <v>8.0877742946708464E-2</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>6.8720000000000003E-2</v>
-          </cell>
-          <cell r="C48">
-            <v>4.3229999999999998E-2</v>
-          </cell>
-          <cell r="D48">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E48">
-            <v>3.1899999999999998E-2</v>
-          </cell>
-          <cell r="L48">
-            <v>7.2100313479623826E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>7.0440000000000003E-2</v>
-          </cell>
-          <cell r="C49">
-            <v>4.7969999999999999E-2</v>
-          </cell>
-          <cell r="D49">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E49">
-            <v>2.1170000000000001E-2</v>
-          </cell>
-          <cell r="L49">
-            <v>6.8965517241379309E-2</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>6.9070000000000006E-2</v>
-          </cell>
-          <cell r="C50">
-            <v>3.0980000000000001E-2</v>
-          </cell>
-          <cell r="D50">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E50">
-            <v>8.8199999999999997E-3</v>
-          </cell>
-          <cell r="L50">
-            <v>4.9529780564263326E-2</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>8.4169999999999995E-2</v>
-          </cell>
-          <cell r="C51">
-            <v>5.629E-2</v>
-          </cell>
-          <cell r="D51">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E51">
-            <v>2.63E-3</v>
-          </cell>
-          <cell r="L51">
-            <v>8.3385579937304069E-2</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>8.183E-2</v>
-          </cell>
-          <cell r="C52">
-            <v>5.8459999999999998E-2</v>
-          </cell>
-          <cell r="D52">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E52">
-            <v>2.82E-3</v>
-          </cell>
-          <cell r="L52">
-            <v>9.7178683385579931E-2</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>7.7030000000000001E-2</v>
-          </cell>
-          <cell r="C53">
-            <v>5.364E-2</v>
-          </cell>
-          <cell r="D53">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E53">
-            <v>2.6970000000000001E-2</v>
-          </cell>
-          <cell r="L53">
-            <v>8.7774294670846395E-2</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>7.9299999999999995E-2</v>
-          </cell>
-          <cell r="C54">
-            <v>6.268E-2</v>
-          </cell>
-          <cell r="D54">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E54">
-            <v>3.3939999999999998E-2</v>
-          </cell>
-          <cell r="L54">
-            <v>0.10219435736677115</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>8.2699999999999996E-2</v>
-          </cell>
-          <cell r="C55">
-            <v>5.6649999999999999E-2</v>
-          </cell>
-          <cell r="D55">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E55">
-            <v>3.49E-3</v>
-          </cell>
-          <cell r="L55">
-            <v>9.6865203761755489E-2</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>8.2199999999999995E-2</v>
-          </cell>
-          <cell r="C56">
-            <v>4.6339999999999999E-2</v>
-          </cell>
-          <cell r="D56">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E56">
-            <v>2.12E-2</v>
-          </cell>
-          <cell r="L56">
-            <v>7.304075235109718E-2</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>7.1940000000000004E-2</v>
-          </cell>
-          <cell r="C57">
-            <v>5.364E-2</v>
-          </cell>
-          <cell r="D57">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E57">
-            <v>1.9720000000000001E-2</v>
-          </cell>
-          <cell r="L57">
-            <v>8.3385579937304069E-2</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58">
-            <v>7.3520000000000002E-2</v>
-          </cell>
-          <cell r="C58">
-            <v>5.8349999999999999E-2</v>
-          </cell>
-          <cell r="D58">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E58">
-            <v>9.6299999999999997E-3</v>
-          </cell>
-          <cell r="L58">
-            <v>9.2476489028213163E-2</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59">
-            <v>7.9200000000000007E-2</v>
-          </cell>
-          <cell r="C59">
-            <v>6.1159999999999999E-2</v>
-          </cell>
-          <cell r="D59">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E59">
-            <v>6.3800000000000003E-3</v>
-          </cell>
-          <cell r="L59">
-            <v>8.9655172413793102E-2</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>7.0300000000000001E-2</v>
-          </cell>
-          <cell r="C60">
-            <v>4.2999999999999997E-2</v>
-          </cell>
-          <cell r="D60">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E60">
-            <v>3.1780000000000003E-2</v>
-          </cell>
-          <cell r="L60">
-            <v>7.0846394984326017E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61">
-            <v>6.9339999999999999E-2</v>
-          </cell>
-          <cell r="C61">
-            <v>3.7130000000000003E-2</v>
-          </cell>
-          <cell r="D61">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E61">
-            <v>3.1559999999999998E-2</v>
-          </cell>
-          <cell r="L61">
-            <v>6.2068965517241378E-2</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62">
-            <v>7.1819999999999995E-2</v>
-          </cell>
-          <cell r="C62">
-            <v>5.398E-2</v>
-          </cell>
-          <cell r="D62">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E62">
-            <v>3.4610000000000002E-2</v>
-          </cell>
-          <cell r="L62">
-            <v>8.2131661442006273E-2</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="B63">
-            <v>6.9440000000000002E-2</v>
-          </cell>
-          <cell r="C63">
-            <v>3.943E-2</v>
-          </cell>
-          <cell r="D63">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E63">
-            <v>3.2680000000000001E-2</v>
-          </cell>
-          <cell r="L63">
-            <v>5.8620689655172413E-2</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64">
-            <v>7.0940000000000003E-2</v>
-          </cell>
-          <cell r="C64">
-            <v>4.462E-2</v>
-          </cell>
-          <cell r="D64">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E64">
-            <v>3.1469999999999998E-2</v>
-          </cell>
-          <cell r="L64">
-            <v>7.304075235109718E-2</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="B65">
-            <v>7.3029999999999998E-2</v>
-          </cell>
-          <cell r="C65">
-            <v>5.3030000000000001E-2</v>
-          </cell>
-          <cell r="D65">
-            <v>6.9999999999999999E-4</v>
-          </cell>
-          <cell r="E65">
-            <v>2.5659999999999999E-2</v>
-          </cell>
-          <cell r="L65">
-            <v>7.7429467084639492E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="B66">
-            <v>7.6530000000000001E-2</v>
-          </cell>
-          <cell r="C66">
-            <v>4.7800000000000002E-2</v>
-          </cell>
-          <cell r="D66">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E66">
-            <v>1.2200000000000001E-2</v>
-          </cell>
-          <cell r="L66">
-            <v>7.6175548589341696E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="B67">
-            <v>7.4910000000000004E-2</v>
-          </cell>
-          <cell r="C67">
-            <v>4.2930000000000003E-2</v>
-          </cell>
-          <cell r="D67">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E67">
-            <v>1.566E-2</v>
-          </cell>
-          <cell r="L67">
-            <v>6.175548589341693E-2</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="B68">
-            <v>7.3929999999999996E-2</v>
-          </cell>
-          <cell r="C68">
-            <v>4.6510000000000003E-2</v>
-          </cell>
-          <cell r="D68">
-            <v>1.0499999999999999E-3</v>
-          </cell>
-          <cell r="E68">
-            <v>7.9900000000000006E-3</v>
-          </cell>
-          <cell r="L68">
-            <v>7.178683385579937E-2</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69">
-            <v>8.4250000000000005E-2</v>
-          </cell>
-          <cell r="C69">
-            <v>6.3519999999999993E-2</v>
-          </cell>
-          <cell r="D69">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E69">
-            <v>2.2919999999999999E-2</v>
-          </cell>
-          <cell r="L69">
-            <v>0.10031347962382445</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="B70">
-            <v>8.0269999999999994E-2</v>
-          </cell>
-          <cell r="C70">
-            <v>5.663E-2</v>
-          </cell>
-          <cell r="D70">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E70">
-            <v>1.1140000000000001E-2</v>
-          </cell>
-          <cell r="L70">
-            <v>9.5924764890282135E-2</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="B71">
-            <v>7.7479999999999993E-2</v>
-          </cell>
-          <cell r="C71">
-            <v>6.173E-2</v>
-          </cell>
-          <cell r="D71">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E71">
-            <v>1.6199999999999999E-2</v>
-          </cell>
-          <cell r="L71">
-            <v>0.10376175548589342</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="B72">
-            <v>8.1350000000000006E-2</v>
-          </cell>
-          <cell r="C72">
-            <v>6.0249999999999998E-2</v>
-          </cell>
-          <cell r="D72">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E72">
-            <v>1.393E-2</v>
-          </cell>
-          <cell r="L72">
-            <v>8.8401253918495293E-2</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73">
-            <v>8.5089999999999999E-2</v>
-          </cell>
-          <cell r="C73">
-            <v>5.7450000000000001E-2</v>
-          </cell>
-          <cell r="D73">
-            <v>6.2E-4</v>
-          </cell>
-          <cell r="E73">
-            <v>1.206E-2</v>
-          </cell>
-          <cell r="L73">
-            <v>9.7492163009404387E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="B74">
-            <v>7.7160000000000006E-2</v>
-          </cell>
-          <cell r="C74">
-            <v>4.9360000000000001E-2</v>
-          </cell>
-          <cell r="D74">
-            <v>6.4999999999999997E-4</v>
-          </cell>
-          <cell r="E74">
-            <v>3.2759999999999997E-2</v>
-          </cell>
-          <cell r="L74">
-            <v>8.2445141065830715E-2</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="B75">
-            <v>8.0909999999999996E-2</v>
-          </cell>
-          <cell r="C75">
-            <v>4.8820000000000002E-2</v>
-          </cell>
-          <cell r="D75">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E75">
-            <v>3.3050000000000003E-2</v>
-          </cell>
-          <cell r="L75">
-            <v>8.0250783699059566E-2</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="B76">
-            <v>7.0669999999999997E-2</v>
-          </cell>
-          <cell r="C76">
-            <v>4.1610000000000001E-2</v>
-          </cell>
-          <cell r="D76">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E76">
-            <v>9.8099999999999993E-3</v>
-          </cell>
-          <cell r="L76">
-            <v>6.9278996865203765E-2</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77">
-            <v>0.10568</v>
-          </cell>
-          <cell r="C77">
-            <v>0.14177000000000001</v>
-          </cell>
-          <cell r="D77">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E77">
-            <v>1.864E-2</v>
-          </cell>
-          <cell r="L77">
-            <v>0.21692789968652038</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78">
-            <v>0.11316</v>
-          </cell>
-          <cell r="C78">
-            <v>0.12728999999999999</v>
-          </cell>
-          <cell r="D78">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E78">
-            <v>1.6999999999999999E-3</v>
-          </cell>
-          <cell r="L78">
-            <v>0.21222570532915361</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79">
-            <v>7.5130000000000002E-2</v>
-          </cell>
-          <cell r="C79">
-            <v>6.8000000000000005E-2</v>
-          </cell>
-          <cell r="D79">
-            <v>5.6999999999999998E-4</v>
-          </cell>
-          <cell r="E79">
-            <v>3.1710000000000002E-2</v>
-          </cell>
-          <cell r="L79">
-            <v>9.3730407523510972E-2</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="B80">
-            <v>7.4990000000000001E-2</v>
-          </cell>
-          <cell r="C80">
-            <v>4.7820000000000001E-2</v>
-          </cell>
-          <cell r="D80">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E80">
-            <v>2.743E-2</v>
-          </cell>
-          <cell r="L80">
-            <v>6.8965517241379309E-2</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="B81">
-            <v>9.7570000000000004E-2</v>
-          </cell>
-          <cell r="C81">
-            <v>0.10244</v>
-          </cell>
-          <cell r="D81">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E81">
-            <v>3.7159999999999999E-2</v>
-          </cell>
-          <cell r="L81">
-            <v>0.16363636363636364</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="B82">
-            <v>8.8569999999999996E-2</v>
-          </cell>
-          <cell r="C82">
-            <v>8.3669999999999994E-2</v>
-          </cell>
-          <cell r="D82">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E82">
-            <v>1.06E-2</v>
-          </cell>
-          <cell r="L82">
-            <v>0.13291536050156741</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83">
-            <v>9.6369999999999997E-2</v>
-          </cell>
-          <cell r="C83">
-            <v>8.7679999999999994E-2</v>
-          </cell>
-          <cell r="D83">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E83">
-            <v>3.295E-2</v>
-          </cell>
-          <cell r="L83">
-            <v>0.13918495297805641</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84">
-            <v>9.5850000000000005E-2</v>
-          </cell>
-          <cell r="C84">
-            <v>0.107</v>
-          </cell>
-          <cell r="D84">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E84">
-            <v>3.2169999999999997E-2</v>
-          </cell>
-          <cell r="L84">
-            <v>0.17648902821316614</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85">
-            <v>9.5329999999999998E-2</v>
-          </cell>
-          <cell r="C85">
-            <v>0.10553999999999999</v>
-          </cell>
-          <cell r="D85">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E85">
-            <v>3.3739999999999999E-2</v>
-          </cell>
-          <cell r="L85">
-            <v>0.16677115987460814</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="B86">
-            <v>9.2869999999999994E-2</v>
-          </cell>
-          <cell r="C86">
-            <v>0.10406</v>
-          </cell>
-          <cell r="D86">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E86">
-            <v>3.2280000000000003E-2</v>
-          </cell>
-          <cell r="L86">
-            <v>0.17523510971786835</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87">
-            <v>9.955E-2</v>
-          </cell>
-          <cell r="C87">
-            <v>0.10113</v>
-          </cell>
-          <cell r="D87">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E87">
-            <v>3.705E-2</v>
-          </cell>
-          <cell r="L87">
-            <v>0.15830721003134796</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88">
-            <v>9.1380000000000003E-2</v>
-          </cell>
-          <cell r="C88">
-            <v>9.8739999999999994E-2</v>
-          </cell>
-          <cell r="D88">
-            <v>6.6E-4</v>
-          </cell>
-          <cell r="E88">
-            <v>2.1389999999999999E-2</v>
-          </cell>
-          <cell r="L88">
-            <v>0.15987460815047022</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="B89">
-            <v>9.6159999999999995E-2</v>
-          </cell>
-          <cell r="C89">
-            <v>9.6610000000000001E-2</v>
-          </cell>
-          <cell r="D89">
-            <v>6.0999999999999997E-4</v>
-          </cell>
-          <cell r="E89">
-            <v>3.8550000000000001E-2</v>
-          </cell>
-          <cell r="L89">
-            <v>0.15862068965517243</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="B90">
-            <v>9.8379999999999995E-2</v>
-          </cell>
-          <cell r="C90">
-            <v>0.10918</v>
-          </cell>
-          <cell r="D90">
-            <v>6.8000000000000005E-4</v>
-          </cell>
-          <cell r="E90">
-            <v>3.1850000000000003E-2</v>
-          </cell>
-          <cell r="L90">
-            <v>0.16990595611285267</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="B91">
-            <v>9.9890000000000007E-2</v>
-          </cell>
-          <cell r="C91">
-            <v>0.10192</v>
-          </cell>
-          <cell r="D91">
-            <v>6.4000000000000005E-4</v>
-          </cell>
-          <cell r="E91">
-            <v>1.1299999999999999E-2</v>
-          </cell>
-          <cell r="L91">
-            <v>0.16708463949843261</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="B92">
-            <v>0.10292999999999999</v>
-          </cell>
-          <cell r="C92">
-            <v>9.6759999999999999E-2</v>
-          </cell>
-          <cell r="D92">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E92">
-            <v>3.6859999999999997E-2</v>
-          </cell>
-          <cell r="L92">
-            <v>0.16175548589341693</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="B93">
-            <v>9.6799999999999997E-2</v>
-          </cell>
-          <cell r="C93">
-            <v>0.10797</v>
-          </cell>
-          <cell r="D93">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E93">
-            <v>3.9199999999999999E-3</v>
-          </cell>
-          <cell r="L93">
-            <v>0.17241379310344829</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="B94">
-            <v>0.10617</v>
-          </cell>
-          <cell r="C94">
-            <v>0.10442</v>
-          </cell>
-          <cell r="D94">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E94">
-            <v>3.415E-2</v>
-          </cell>
-          <cell r="L94">
-            <v>0.16175548589341693</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="B95">
-            <v>9.7689999999999999E-2</v>
-          </cell>
-          <cell r="C95">
-            <v>0.10664</v>
-          </cell>
-          <cell r="D95">
-            <v>6.9999999999999999E-4</v>
-          </cell>
-          <cell r="E95">
-            <v>3.295E-2</v>
-          </cell>
-          <cell r="L95">
-            <v>0.15485893416927898</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="B96">
-            <v>0.10465000000000001</v>
-          </cell>
-          <cell r="C96">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="D96">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E96">
-            <v>1.482E-2</v>
-          </cell>
-          <cell r="L96">
-            <v>0.1683385579937304</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="B97">
-            <v>8.5830000000000004E-2</v>
-          </cell>
-          <cell r="C97">
-            <v>9.3770000000000006E-2</v>
-          </cell>
-          <cell r="D97">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E97">
-            <v>2.1059999999999999E-2</v>
-          </cell>
-          <cell r="L97">
-            <v>0.14514106583072101</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="B98">
-            <v>0.10596</v>
-          </cell>
-          <cell r="C98">
-            <v>9.2670000000000002E-2</v>
-          </cell>
-          <cell r="D98">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E98">
-            <v>2.9489999999999999E-2</v>
-          </cell>
-          <cell r="L98">
-            <v>0.16144200626959249</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="B99">
-            <v>9.6579999999999999E-2</v>
-          </cell>
-          <cell r="C99">
-            <v>9.0789999999999996E-2</v>
-          </cell>
-          <cell r="D99">
-            <v>5.8E-4</v>
-          </cell>
-          <cell r="E99">
-            <v>3.3149999999999999E-2</v>
-          </cell>
-          <cell r="L99">
-            <v>0.15391849529780563</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="B100">
-            <v>0.10127</v>
-          </cell>
-          <cell r="C100">
-            <v>9.2369999999999994E-2</v>
-          </cell>
-          <cell r="D100">
-            <v>5.9000000000000003E-4</v>
-          </cell>
-          <cell r="E100">
-            <v>3.2500000000000001E-2</v>
-          </cell>
-          <cell r="L100">
-            <v>0.15830721003134796</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="B101">
-            <v>0.1016</v>
-          </cell>
-          <cell r="C101">
-            <v>9.8129999999999995E-2</v>
-          </cell>
-          <cell r="D101">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E101">
-            <v>1.9879999999999998E-2</v>
-          </cell>
-          <cell r="L101">
-            <v>0.15987460815047022</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="B102">
-            <v>9.5219999999999999E-2</v>
-          </cell>
-          <cell r="C102">
-            <v>9.6909999999999996E-2</v>
-          </cell>
-          <cell r="D102">
-            <v>7.1000000000000002E-4</v>
-          </cell>
-          <cell r="E102">
-            <v>1.5259999999999999E-2</v>
-          </cell>
-          <cell r="L102">
-            <v>0.15956112852664578</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="B103">
-            <v>9.7839999999999996E-2</v>
-          </cell>
-          <cell r="C103">
-            <v>0.10372000000000001</v>
-          </cell>
-          <cell r="D103">
-            <v>6.8999999999999997E-4</v>
-          </cell>
-          <cell r="E103">
-            <v>3.209E-2</v>
-          </cell>
-          <cell r="L103">
-            <v>0.16269592476489028</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="B104">
-            <v>9.6920000000000006E-2</v>
-          </cell>
-          <cell r="C104">
-            <v>9.8489999999999994E-2</v>
-          </cell>
-          <cell r="D104">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-          <cell r="E104">
-            <v>3.3070000000000002E-2</v>
-          </cell>
-          <cell r="L104">
-            <v>0.16269592476489028</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="B105">
-            <v>9.4640000000000002E-2</v>
-          </cell>
-          <cell r="C105">
-            <v>9.9040000000000003E-2</v>
-          </cell>
-          <cell r="D105">
-            <v>6.3000000000000003E-4</v>
-          </cell>
-          <cell r="E105">
-            <v>3.3009999999999998E-2</v>
-          </cell>
-          <cell r="L105">
-            <v>0.1542319749216301</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9952,7 +6546,7 @@
   <dimension ref="A1:L105"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B105"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>